<commit_message>
Add data_format field to DownloadableFiles model
</commit_message>
<xml_diff>
--- a/tests/services/data/pbmc_invalid.xlsx
+++ b/tests/services/data/pbmc_invalid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-api-gae/tests/services/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3D7F3BF-636B-F64A-8DA7-81CF9CE8F9A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF1778C7-B67C-094B-8CBF-385D864A664A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50780" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="23760" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBMCs" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+          <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
         </r>
       </text>
     </comment>
@@ -164,7 +164,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Courier account number to pay for shipping if avaialable. Example: 45465732.</t>
+          <t>Courier account number to pay for shipping if available. Example: 45465732.</t>
         </r>
       </text>
     </comment>
@@ -177,7 +177,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Type of shippment made.</t>
+          <t>Type of shipment made.</t>
         </r>
       </text>
     </comment>
@@ -268,7 +268,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+          <t>Trial Participant Identifier. Example: PT123.</t>
         </r>
       </text>
     </comment>
@@ -281,7 +281,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial Participant Identifier. Example: PT123.</t>
+          <t>Participant identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-1234.</t>
         </r>
       </text>
     </comment>
@@ -294,7 +294,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Participant identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-1234.</t>
+          <t>Identifies the treatment cohort to which the participant belongs. Example: Cohort A.</t>
         </r>
       </text>
     </comment>
@@ -307,7 +307,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Identifies the treatment cohort to which the participant belongs. Example: Cohort A.</t>
+          <t>Identifies the trial arm to which the participant belongs. Example: Arm A.</t>
         </r>
       </text>
     </comment>
@@ -320,7 +320,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Identifies the trial arm to which the participant belongs. Example: Arm A.</t>
+          <t>Sample identifier assigned by the biorepository site. Example: EA123-45.</t>
         </r>
       </text>
     </comment>
@@ -333,7 +333,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sample identifier assigned by the biorepository site. Example: EA123-45.</t>
+          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
         </r>
       </text>
     </comment>
@@ -346,7 +346,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
+          <t>Study related collection time point, as described in the protocol intake form. Example: Progression.</t>
         </r>
       </text>
     </comment>
@@ -359,7 +359,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Study related collection time point, as described in the protocol intake form. Example: Progression.</t>
+          <t>Date of blood collection.</t>
         </r>
       </text>
     </comment>
@@ -372,7 +372,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of blood collection.</t>
+          <t>Time of blood collection.</t>
         </r>
       </text>
     </comment>
@@ -385,7 +385,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time of blood collection.</t>
+          <t>Date of blood processing.</t>
         </r>
       </text>
     </comment>
@@ -398,7 +398,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of blood processing.</t>
+          <t>Time of blood processing.</t>
         </r>
       </text>
     </comment>
@@ -411,7 +411,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time of blood processing.</t>
+          <t>Sample location within the shipping container. Example: A1.</t>
         </r>
       </text>
     </comment>
@@ -424,7 +424,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sample location within the shipping container. Example: A1.</t>
+          <t>Type of sample sent.</t>
         </r>
       </text>
     </comment>
@@ -437,7 +437,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Type of sample sent.</t>
+          <t>The format in which the sample was sent.</t>
         </r>
       </text>
     </comment>
@@ -450,7 +450,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The format in which the sample was sent.</t>
+          <t>Quantity of each aliquot shipped.</t>
         </r>
       </text>
     </comment>
@@ -463,7 +463,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Quantity of each sample shipped.</t>
+          <t>Volume of aliquot shipped.</t>
         </r>
       </text>
     </comment>
@@ -476,7 +476,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Volume of sample shipped.</t>
+          <t>The unit of biological material from this aliquot.</t>
         </r>
       </text>
     </comment>
@@ -489,7 +489,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Unit of each sample. Example: ml.</t>
+          <t>Site or biobank provides the final number of PBMCs per vial that were frozen.</t>
         </r>
       </text>
     </comment>
@@ -502,7 +502,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Site or biobank provides the final number of PBMCs per vial that were frozen.</t>
+          <t>Indicates the specimen source of the sample shipped. Example: Na Heparin blood draw aliquots (2 of three), FFPE block #52</t>
         </r>
       </text>
     </comment>
@@ -515,7 +515,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Indicates the specimen source of the sample shipped. Example: Na Heparin blood draw aliquots (2 of three), FFPE block #52</t>
+          <t>Aliquot identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
         </r>
       </text>
     </comment>
@@ -528,7 +528,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Aliquot identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
+          <t>Receiving site determines number fo PBMCs per vial recovered upon receipt.</t>
         </r>
       </text>
     </comment>
@@ -541,7 +541,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site determines number fo PBMCs per vial recovered upon receipt.</t>
+          <t>Receiving site indicates how much material was used for assay purposes.</t>
         </r>
       </text>
     </comment>
@@ -554,7 +554,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site indicates how much material was used for assay purposes.</t>
+          <t>Receiving site indicates how much material remains after assay use.</t>
         </r>
       </text>
     </comment>
@@ -567,7 +567,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site indicates how much material remains after assay use.</t>
+          <t>Final status of aliquot after QC and pathology review.</t>
         </r>
       </text>
     </comment>
@@ -580,7 +580,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Final status of sample after QC and pathology review.</t>
+          <t>Status of aliquot if replacement is/was requested.</t>
         </r>
       </text>
     </comment>
@@ -593,20 +593,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Status of sample if replacement is/was requested.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AB22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Status of sample used for other assay, exhausted, destroyed, or returned.</t>
+          <t>Status of aliquot used for other assay, exhausted, destroyed, or returned.</t>
         </r>
       </text>
     </comment>
@@ -615,7 +602,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="75">
   <si>
     <t>#t</t>
   </si>
@@ -776,6 +763,9 @@
     <t>Assay-5</t>
   </si>
   <si>
+    <t>Green-top Tube - Plasma (Olink)</t>
+  </si>
+  <si>
     <t>USPS</t>
   </si>
   <si>
@@ -794,6 +784,9 @@
     <t>DFCI</t>
   </si>
   <si>
+    <t xml:space="preserve">Baseline </t>
+  </si>
+  <si>
     <t>A1</t>
   </si>
   <si>
@@ -803,7 +796,7 @@
     <t>EDTA Tube</t>
   </si>
   <si>
-    <t>ml</t>
+    <t>mL</t>
   </si>
   <si>
     <t>FFPE block #52</t>
@@ -812,31 +805,28 @@
     <t>CIMAC-12345</t>
   </si>
   <si>
+    <t>CIMAC-45678</t>
+  </si>
+  <si>
+    <t>CIMAC-54321</t>
+  </si>
+  <si>
+    <t>CIMAC-12354</t>
+  </si>
+  <si>
+    <t>CIMAC-12435</t>
+  </si>
+  <si>
+    <t>CIMAC-14345</t>
+  </si>
+  <si>
     <t>Usable for Assay</t>
   </si>
   <si>
     <t>Replacement Tested</t>
   </si>
   <si>
-    <t>Sample Exhausted</t>
-  </si>
-  <si>
-    <t>CIMAC-45678</t>
-  </si>
-  <si>
-    <t>CIMAC-54321</t>
-  </si>
-  <si>
-    <t>CIMAC-12354</t>
-  </si>
-  <si>
-    <t>CIMAC-12435</t>
-  </si>
-  <si>
-    <t>CIMAC-14345</t>
-  </si>
-  <si>
-    <t>blah blah blah</t>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -930,7 +920,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -942,6 +932,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1284,10 +1275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB222"/>
+  <dimension ref="A1:AA222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23:O28"/>
+    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1296,41 +1287,40 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-    </row>
-    <row r="2" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+    </row>
+    <row r="2" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1364,9 +1354,8 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-    </row>
-    <row r="3" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1400,9 +1389,8 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-    </row>
-    <row r="4" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1436,9 +1424,8 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-    </row>
-    <row r="5" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1472,16 +1459,17 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-    </row>
-    <row r="6" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1506,9 +1494,8 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-    </row>
-    <row r="7" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1542,9 +1529,8 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-    </row>
-    <row r="8" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1578,16 +1564,17 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-    </row>
-    <row r="9" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <v>123</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1612,9 +1599,8 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-    </row>
-    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1622,7 +1608,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1648,9 +1634,8 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-    </row>
-    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1658,7 +1643,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1684,9 +1669,8 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-    </row>
-    <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1694,7 +1678,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1720,9 +1704,8 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-    </row>
-    <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1730,7 +1713,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1756,9 +1739,8 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-    </row>
-    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1792,9 +1774,8 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-    </row>
-    <row r="15" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1828,9 +1809,8 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-    </row>
-    <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1864,9 +1844,8 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-    </row>
-    <row r="17" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1900,9 +1879,8 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-    </row>
-    <row r="18" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1910,7 +1888,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1936,9 +1914,8 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
-    </row>
-    <row r="19" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1946,7 +1923,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1972,659 +1949,633 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B21" s="6" t="s">
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6" t="s">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="W21" s="6"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="6"/>
-      <c r="AA21" s="6"/>
-      <c r="AB21" s="6"/>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7"/>
+      <c r="AA21" s="7"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Z22" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AA22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB22" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23">
+        <v>54321</v>
+      </c>
+      <c r="C23">
         <v>12345</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>54321</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>12345</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>54321</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>12345</v>
       </c>
-      <c r="G23">
-        <v>54321</v>
-      </c>
-      <c r="H23">
-        <v>12345</v>
-      </c>
-      <c r="I23" s="4">
-        <v>0.42444444444444446</v>
+      <c r="H23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I23" s="6">
+        <v>33234</v>
       </c>
       <c r="J23" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K23">
         <v>41193</v>
       </c>
-      <c r="K23" s="4">
-        <v>0.42444444444444446</v>
-      </c>
       <c r="L23" s="5">
-        <v>41193</v>
-      </c>
-      <c r="M23" s="4">
-        <v>0.42444444444444446</v>
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M23" t="s">
+        <v>61</v>
       </c>
       <c r="N23" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="O23" t="s">
-        <v>73</v>
-      </c>
-      <c r="P23" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="P23">
+        <v>100</v>
       </c>
       <c r="Q23">
         <v>100</v>
       </c>
-      <c r="R23">
+      <c r="R23" t="s">
+        <v>64</v>
+      </c>
+      <c r="S23">
+        <v>10</v>
+      </c>
+      <c r="T23" t="s">
+        <v>65</v>
+      </c>
+      <c r="U23" t="s">
+        <v>66</v>
+      </c>
+      <c r="V23">
+        <v>123</v>
+      </c>
+      <c r="W23">
+        <v>122</v>
+      </c>
+      <c r="X23">
         <v>100</v>
       </c>
-      <c r="S23" t="s">
+      <c r="Y23" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>54321</v>
+      </c>
+      <c r="C24">
+        <v>12345</v>
+      </c>
+      <c r="D24">
+        <v>54321</v>
+      </c>
+      <c r="E24">
+        <v>12345</v>
+      </c>
+      <c r="F24">
+        <v>54321</v>
+      </c>
+      <c r="G24">
+        <v>12345</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="6">
+        <v>33234</v>
+      </c>
+      <c r="J24" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K24">
+        <v>41193</v>
+      </c>
+      <c r="L24" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M24" t="s">
+        <v>61</v>
+      </c>
+      <c r="N24" t="s">
         <v>62</v>
       </c>
-      <c r="T23">
-        <v>10</v>
-      </c>
-      <c r="U23" t="s">
+      <c r="O24" t="s">
         <v>63</v>
       </c>
-      <c r="V23" t="s">
-        <v>64</v>
-      </c>
-      <c r="W23">
-        <v>123</v>
-      </c>
-      <c r="X23">
-        <v>122</v>
-      </c>
-      <c r="Y23">
+      <c r="P24">
         <v>100</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24">
-        <v>12345</v>
-      </c>
-      <c r="C24">
-        <v>54321</v>
-      </c>
-      <c r="D24">
-        <v>12345</v>
-      </c>
-      <c r="E24">
-        <v>54321</v>
-      </c>
-      <c r="F24">
-        <v>12345</v>
-      </c>
-      <c r="G24">
-        <v>54321</v>
-      </c>
-      <c r="H24">
-        <v>12345</v>
-      </c>
-      <c r="I24" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="J24" t="s">
-        <v>65</v>
-      </c>
-      <c r="K24" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="L24" s="5">
-        <v>41193</v>
-      </c>
-      <c r="M24" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="N24" t="s">
-        <v>59</v>
-      </c>
-      <c r="O24" t="s">
-        <v>60</v>
-      </c>
-      <c r="P24" t="s">
-        <v>61</v>
       </c>
       <c r="Q24">
         <v>100</v>
       </c>
-      <c r="R24">
+      <c r="R24" t="s">
+        <v>64</v>
+      </c>
+      <c r="S24">
+        <v>10</v>
+      </c>
+      <c r="T24" t="s">
+        <v>65</v>
+      </c>
+      <c r="U24" t="s">
+        <v>67</v>
+      </c>
+      <c r="V24">
+        <v>123</v>
+      </c>
+      <c r="W24">
+        <v>122</v>
+      </c>
+      <c r="X24">
         <v>100</v>
       </c>
-      <c r="S24" t="s">
+      <c r="Y24" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>54321</v>
+      </c>
+      <c r="C25">
+        <v>12345</v>
+      </c>
+      <c r="D25">
+        <v>54321</v>
+      </c>
+      <c r="E25">
+        <v>12345</v>
+      </c>
+      <c r="F25">
+        <v>54321</v>
+      </c>
+      <c r="G25">
+        <v>12345</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J25" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L25" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M25" t="s">
+        <v>61</v>
+      </c>
+      <c r="N25" t="s">
         <v>62</v>
       </c>
-      <c r="T24">
-        <v>10</v>
-      </c>
-      <c r="U24" t="s">
+      <c r="O25" t="s">
         <v>63</v>
       </c>
-      <c r="V24" t="s">
-        <v>68</v>
-      </c>
-      <c r="W24">
-        <v>123</v>
-      </c>
-      <c r="X24">
-        <v>122</v>
-      </c>
-      <c r="Y24">
+      <c r="P25">
         <v>100</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>12345</v>
-      </c>
-      <c r="C25">
-        <v>54321</v>
-      </c>
-      <c r="D25">
-        <v>12345</v>
-      </c>
-      <c r="E25">
-        <v>54321</v>
-      </c>
-      <c r="F25">
-        <v>12345</v>
-      </c>
-      <c r="G25">
-        <v>54321</v>
-      </c>
-      <c r="H25">
-        <v>12345</v>
-      </c>
-      <c r="I25" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="J25" s="5">
-        <v>41193</v>
-      </c>
-      <c r="K25" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="L25" s="5">
-        <v>41193</v>
-      </c>
-      <c r="M25" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="N25" t="s">
-        <v>59</v>
-      </c>
-      <c r="O25" t="s">
-        <v>60</v>
-      </c>
-      <c r="P25" t="s">
-        <v>61</v>
       </c>
       <c r="Q25">
         <v>100</v>
       </c>
-      <c r="R25">
+      <c r="R25" t="s">
+        <v>64</v>
+      </c>
+      <c r="S25">
+        <v>10</v>
+      </c>
+      <c r="T25" t="s">
+        <v>65</v>
+      </c>
+      <c r="U25" t="s">
+        <v>68</v>
+      </c>
+      <c r="V25">
+        <v>123</v>
+      </c>
+      <c r="W25">
+        <v>122</v>
+      </c>
+      <c r="X25">
         <v>100</v>
       </c>
-      <c r="S25" t="s">
+      <c r="Y25" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>54321</v>
+      </c>
+      <c r="C26">
+        <v>12345</v>
+      </c>
+      <c r="D26">
+        <v>54321</v>
+      </c>
+      <c r="E26">
+        <v>12345</v>
+      </c>
+      <c r="F26">
+        <v>54321</v>
+      </c>
+      <c r="G26">
+        <v>12345</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I26" s="6">
+        <v>33234</v>
+      </c>
+      <c r="J26" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K26">
+        <v>41193</v>
+      </c>
+      <c r="L26" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M26" t="s">
+        <v>61</v>
+      </c>
+      <c r="N26" t="s">
         <v>62</v>
       </c>
-      <c r="T25">
-        <v>10</v>
-      </c>
-      <c r="U25" t="s">
+      <c r="O26" t="s">
         <v>63</v>
       </c>
-      <c r="V25" t="s">
-        <v>69</v>
-      </c>
-      <c r="W25">
-        <v>123</v>
-      </c>
-      <c r="X25">
-        <v>122</v>
-      </c>
-      <c r="Y25">
+      <c r="P26">
         <v>100</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>12345</v>
-      </c>
-      <c r="C26">
-        <v>54321</v>
-      </c>
-      <c r="D26">
-        <v>12345</v>
-      </c>
-      <c r="E26">
-        <v>54321</v>
-      </c>
-      <c r="F26">
-        <v>12345</v>
-      </c>
-      <c r="G26">
-        <v>54321</v>
-      </c>
-      <c r="H26">
-        <v>12345</v>
-      </c>
-      <c r="I26" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="J26" s="5">
-        <v>41193</v>
-      </c>
-      <c r="K26" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="L26" s="5">
-        <v>41193</v>
-      </c>
-      <c r="M26" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="N26" t="s">
-        <v>59</v>
-      </c>
-      <c r="O26" t="s">
-        <v>60</v>
-      </c>
-      <c r="P26" t="s">
-        <v>61</v>
       </c>
       <c r="Q26">
         <v>100</v>
       </c>
-      <c r="R26">
+      <c r="R26" t="s">
+        <v>64</v>
+      </c>
+      <c r="S26">
+        <v>10</v>
+      </c>
+      <c r="T26" t="s">
+        <v>65</v>
+      </c>
+      <c r="U26" t="s">
+        <v>69</v>
+      </c>
+      <c r="V26">
+        <v>123</v>
+      </c>
+      <c r="W26">
+        <v>122</v>
+      </c>
+      <c r="X26">
         <v>100</v>
       </c>
-      <c r="S26" t="s">
+      <c r="Y26" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>54321</v>
+      </c>
+      <c r="C27">
+        <v>12345</v>
+      </c>
+      <c r="D27">
+        <v>54321</v>
+      </c>
+      <c r="E27">
+        <v>12345</v>
+      </c>
+      <c r="F27">
+        <v>54321</v>
+      </c>
+      <c r="G27">
+        <v>12345</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" s="6">
+        <v>33234</v>
+      </c>
+      <c r="J27" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K27">
+        <v>41193</v>
+      </c>
+      <c r="L27" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M27" t="s">
+        <v>61</v>
+      </c>
+      <c r="N27" t="s">
         <v>62</v>
       </c>
-      <c r="T26">
-        <v>10</v>
-      </c>
-      <c r="U26" t="s">
+      <c r="O27" t="s">
         <v>63</v>
       </c>
-      <c r="V26" t="s">
-        <v>70</v>
-      </c>
-      <c r="W26">
-        <v>123</v>
-      </c>
-      <c r="X26">
-        <v>122</v>
-      </c>
-      <c r="Y26">
+      <c r="P27">
         <v>100</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27">
-        <v>12345</v>
-      </c>
-      <c r="C27">
-        <v>54321</v>
-      </c>
-      <c r="D27">
-        <v>12345</v>
-      </c>
-      <c r="E27">
-        <v>54321</v>
-      </c>
-      <c r="F27">
-        <v>12345</v>
-      </c>
-      <c r="G27">
-        <v>54321</v>
-      </c>
-      <c r="H27">
-        <v>12345</v>
-      </c>
-      <c r="I27" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="J27" s="5">
-        <v>41193</v>
-      </c>
-      <c r="K27" t="s">
-        <v>72</v>
-      </c>
-      <c r="L27" s="5">
-        <v>41193</v>
-      </c>
-      <c r="M27" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="N27" t="s">
-        <v>59</v>
-      </c>
-      <c r="O27" t="s">
-        <v>60</v>
-      </c>
-      <c r="P27" t="s">
-        <v>61</v>
       </c>
       <c r="Q27">
         <v>100</v>
       </c>
-      <c r="R27">
+      <c r="R27" t="s">
+        <v>64</v>
+      </c>
+      <c r="S27">
+        <v>10</v>
+      </c>
+      <c r="T27" t="s">
+        <v>65</v>
+      </c>
+      <c r="U27" t="s">
+        <v>70</v>
+      </c>
+      <c r="V27">
+        <v>123</v>
+      </c>
+      <c r="W27">
+        <v>122</v>
+      </c>
+      <c r="X27">
         <v>100</v>
       </c>
-      <c r="S27" t="s">
+      <c r="Y27" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>54321</v>
+      </c>
+      <c r="C28">
+        <v>12345</v>
+      </c>
+      <c r="D28">
+        <v>54321</v>
+      </c>
+      <c r="E28">
+        <v>12345</v>
+      </c>
+      <c r="F28">
+        <v>54321</v>
+      </c>
+      <c r="G28">
+        <v>12345</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I28" s="6">
+        <v>33234</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K28">
+        <v>41193</v>
+      </c>
+      <c r="L28" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M28" t="s">
+        <v>61</v>
+      </c>
+      <c r="N28" t="s">
         <v>62</v>
       </c>
-      <c r="T27">
-        <v>10</v>
-      </c>
-      <c r="U27" t="s">
+      <c r="O28" t="s">
         <v>63</v>
       </c>
-      <c r="V27" t="s">
-        <v>71</v>
-      </c>
-      <c r="W27">
-        <v>123</v>
-      </c>
-      <c r="X27">
-        <v>122</v>
-      </c>
-      <c r="Y27">
+      <c r="P28">
         <v>100</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28">
-        <v>12345</v>
-      </c>
-      <c r="C28">
-        <v>54321</v>
-      </c>
-      <c r="D28">
-        <v>12345</v>
-      </c>
-      <c r="E28">
-        <v>54321</v>
-      </c>
-      <c r="F28">
-        <v>12345</v>
-      </c>
-      <c r="G28">
-        <v>54321</v>
-      </c>
-      <c r="H28">
-        <v>12345</v>
-      </c>
-      <c r="I28" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="J28" s="5">
-        <v>41193</v>
-      </c>
-      <c r="K28" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="L28" s="5">
-        <v>41193</v>
-      </c>
-      <c r="M28" s="4">
-        <v>0.42444444444444446</v>
-      </c>
-      <c r="N28" t="s">
-        <v>59</v>
-      </c>
-      <c r="O28" t="s">
-        <v>60</v>
-      </c>
-      <c r="P28" t="s">
-        <v>61</v>
       </c>
       <c r="Q28">
         <v>100</v>
       </c>
-      <c r="R28">
+      <c r="R28" t="s">
+        <v>64</v>
+      </c>
+      <c r="S28">
+        <v>10</v>
+      </c>
+      <c r="T28" t="s">
+        <v>65</v>
+      </c>
+      <c r="U28" t="s">
+        <v>71</v>
+      </c>
+      <c r="V28">
+        <v>123</v>
+      </c>
+      <c r="W28">
+        <v>122</v>
+      </c>
+      <c r="X28">
         <v>100</v>
       </c>
-      <c r="S28" t="s">
-        <v>62</v>
-      </c>
-      <c r="T28">
-        <v>10</v>
-      </c>
-      <c r="U28" t="s">
-        <v>63</v>
-      </c>
-      <c r="V28" t="s">
+      <c r="Y28" t="s">
         <v>72</v>
       </c>
-      <c r="W28">
-        <v>123</v>
-      </c>
-      <c r="X28">
-        <v>122</v>
-      </c>
-      <c r="Y28">
-        <v>100</v>
-      </c>
       <c r="Z28" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="AA28" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -3581,44 +3532,50 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:AB1"/>
+    <mergeCell ref="B1:AA1"/>
     <mergeCell ref="B21:U21"/>
-    <mergeCell ref="V21:AB21"/>
+    <mergeCell ref="V21:AA21"/>
   </mergeCells>
-  <dataValidations count="11">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{E740EEFD-BA74-6847-9464-C02DCACF9945}">
+  <dataValidations count="13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{F3E6FE57-72BC-A740-8715-EFC67E4B4A18}">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{CF43E531-8BC8-6A4D-A70A-F0BC18081BCC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{CF5C08EF-F396-B04E-BDB1-A22098E080AA}">
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{4C550642-C2DB-FC4B-AC4E-887CEC51F5F4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{D6766716-97CD-D448-8D73-8476497F5B74}">
       <formula1>"Frozen (Dry Ice),Frozen (Dry Shipper),Ambient (Ice Pack),Ambient,Other"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{50BA3003-5FF9-B345-9EF8-405B6D32D78A}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{9BC69022-A0AD-C645-82ED-2DA1E8EE9692}">
       <formula1>AND(ISNUMBER(C14),LEFT(CELL("format",C14),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="L23:L222 J25:J222 J23" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>AND(ISNUMBER(J23:J222),LEFT(CELL("format",J23:J222),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="I26:I222 I23:I24 K23:K24 K26:K222" xr:uid="{00000000-0002-0000-0000-000004000000}">
+      <formula1>AND(ISNUMBER(I23:I222),LEFT(CELL("format",I23:I222),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="M23:M222 K28:K222 K23:K26" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L23:L222 J23:J27 J29:J222" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O24:O222" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N23:N222" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"Core Needle Biopsy,Surgical Resection,Endoscopic Biopsy,Punch Biopsy,Plasma,PBMC,Whole Blood,Stool Sample,Bone Marrow Aspirate,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P23:P222" xr:uid="{00000000-0002-0000-0000-000009000000}">
-      <formula1>"FFPE Block,FFPE Scroll,FFPE Core Punch,Unstained Slide,Frozen Tissue,Sodium Heparin Green-Top Tube,Streck Tube,EDTA Tube,Archival FFPE Block,Archival FFPE Slides,Archival FFPE Core Punch,Archival FFPE Scroll,Other,Frozen Stool,DNA-Preserved Stool,Other"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O23:O222" xr:uid="{00000000-0002-0000-0000-000009000000}">
+      <formula1>"FFPE Block,FFPE Scroll,FFPE Core Punch,Unstained Slide,Frozen Tissue,Sodium Heparin Green-Top Tube,Streck Tube,EDTA Tube,Archival FFPE Block,Archival FFPE Slides,Archival FFPE Core Punch,Archival FFPE Scroll,Frozen Stool,DNA-Preserved Stool,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z23:Z222 J24" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R23:R222" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+      <formula1>"µL,mL,mg,ng,Vials,Slides,Scrolls,Blocks,ng/µL,cells/ml,N/A,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y23:Y222" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA23:AA222" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z23:Z222" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB23:AB222" xr:uid="{00000000-0002-0000-0000-00000C000000}">
-      <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA29:AA222" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+      <formula1>"Aliquot Returned,Aliquot Exhausted,Remainder used for other Assay,Other,Aliquot Leftover"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA23:AA28" xr:uid="{984A6193-A151-A644-8F31-8366A7AFC467}">
+      <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other,Sample Leftover"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>